<commit_message>
06/11/2025, Francesco chiede di usare sempre il 1° foglio presente nel file, indipendentemente dal nome
</commit_message>
<xml_diff>
--- a/AAA Files for demo/Input files/Superdettagli_Light.xlsx
+++ b/AAA Files for demo/Input files/Superdettagli_Light.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\Lefo\Dev\3 GDPptGenerator\Solution\FilesEditor.Tests\TestFiles\SourceFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E248AF3-43E5-42FB-85E1-3CC6DD2C7176}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C936614A-0D06-4588-A10B-BB233A8EB351}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Superdetails" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -970,9 +970,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BH13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Renaming Introduzione Singleton per Eppluls helpes Ottimizazioni su import superdettagli
</commit_message>
<xml_diff>
--- a/AAA Files for demo/Input files/Superdettagli_Light.xlsx
+++ b/AAA Files for demo/Input files/Superdettagli_Light.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\Lefo\Dev\3 GDPptGenerator\Solution\FilesEditor.Tests\TestFiles\SourceFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\Lefo\Dev\3 GDPptGenerator\AAA Files for demo\Input files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15C103FD-D92B-4CA3-8764-AC6847A80D37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9FD345B-B72F-423F-8112-9EEE61D29BF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="185">
   <si>
     <t>E005RD002</t>
   </si>
@@ -555,6 +555,42 @@
   </si>
   <si>
     <t>Data Uscita GD</t>
+  </si>
+  <si>
+    <t>New 1</t>
+  </si>
+  <si>
+    <t>New 2</t>
+  </si>
+  <si>
+    <t>New 3</t>
+  </si>
+  <si>
+    <t>New 4</t>
+  </si>
+  <si>
+    <t>New 5</t>
+  </si>
+  <si>
+    <t>New 6</t>
+  </si>
+  <si>
+    <t>New 7</t>
+  </si>
+  <si>
+    <t>New 8</t>
+  </si>
+  <si>
+    <t>New 9</t>
+  </si>
+  <si>
+    <t>New 10</t>
+  </si>
+  <si>
+    <t>New 11</t>
+  </si>
+  <si>
+    <t>New 12</t>
   </si>
 </sst>
 </file>
@@ -694,9 +730,9 @@
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -987,7 +1023,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AY13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1192,8 +1230,8 @@
       <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3">
-        <v>1598</v>
+      <c r="C2" s="3" t="s">
+        <v>173</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>2</v>
@@ -1341,8 +1379,8 @@
       <c r="B3" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="4">
-        <v>1598</v>
+      <c r="C3" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>32</v>
@@ -1490,8 +1528,8 @@
       <c r="B4" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C4" s="3">
-        <v>1598</v>
+      <c r="C4" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>46</v>
@@ -1639,8 +1677,8 @@
       <c r="B5" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C5" s="4">
-        <v>1598</v>
+      <c r="C5" s="3" t="s">
+        <v>176</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>56</v>
@@ -1788,8 +1826,8 @@
       <c r="B6" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C6" s="3">
-        <v>1598</v>
+      <c r="C6" s="3" t="s">
+        <v>177</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>46</v>
@@ -1937,8 +1975,8 @@
       <c r="B7" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C7" s="4">
-        <v>1598</v>
+      <c r="C7" s="3" t="s">
+        <v>178</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>56</v>
@@ -2086,8 +2124,8 @@
       <c r="B8" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="3">
-        <v>1598</v>
+      <c r="C8" s="3" t="s">
+        <v>179</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>86</v>
@@ -2235,8 +2273,8 @@
       <c r="B9" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C9" s="4">
-        <v>1598</v>
+      <c r="C9" s="3" t="s">
+        <v>180</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>92</v>
@@ -2384,8 +2422,8 @@
       <c r="B10" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C10" s="3">
-        <v>1598</v>
+      <c r="C10" s="3" t="s">
+        <v>181</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>46</v>
@@ -2533,8 +2571,8 @@
       <c r="B11" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="4">
-        <v>1598</v>
+      <c r="C11" s="3" t="s">
+        <v>182</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>105</v>
@@ -2682,8 +2720,8 @@
       <c r="B12" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="C12" s="3">
-        <v>1598</v>
+      <c r="C12" s="3" t="s">
+        <v>183</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>56</v>
@@ -2831,8 +2869,8 @@
       <c r="B13" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="2">
-        <v>1598</v>
+      <c r="C13" s="3" t="s">
+        <v>184</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>46</v>

</xml_diff>

<commit_message>
Refactoring con Cancellarzione e inserimento righe in modo massimo
</commit_message>
<xml_diff>
--- a/AAA Files for demo/Input files/Superdettagli_Light.xlsx
+++ b/AAA Files for demo/Input files/Superdettagli_Light.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\Lefo\Dev\3 GDPptGenerator\AAA Files for demo\Input files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\Lefo\Dev\3 GDPptGenerator\Solution\FilesEditor.Tests\TestFiles\SourceFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9FD345B-B72F-423F-8112-9EEE61D29BF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15C103FD-D92B-4CA3-8764-AC6847A80D37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="173">
   <si>
     <t>E005RD002</t>
   </si>
@@ -555,42 +555,6 @@
   </si>
   <si>
     <t>Data Uscita GD</t>
-  </si>
-  <si>
-    <t>New 1</t>
-  </si>
-  <si>
-    <t>New 2</t>
-  </si>
-  <si>
-    <t>New 3</t>
-  </si>
-  <si>
-    <t>New 4</t>
-  </si>
-  <si>
-    <t>New 5</t>
-  </si>
-  <si>
-    <t>New 6</t>
-  </si>
-  <si>
-    <t>New 7</t>
-  </si>
-  <si>
-    <t>New 8</t>
-  </si>
-  <si>
-    <t>New 9</t>
-  </si>
-  <si>
-    <t>New 10</t>
-  </si>
-  <si>
-    <t>New 11</t>
-  </si>
-  <si>
-    <t>New 12</t>
   </si>
 </sst>
 </file>
@@ -730,9 +694,9 @@
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1023,9 +987,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AY13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1230,8 +1192,8 @@
       <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>173</v>
+      <c r="C2" s="3">
+        <v>1598</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>2</v>
@@ -1379,8 +1341,8 @@
       <c r="B3" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>174</v>
+      <c r="C3" s="4">
+        <v>1598</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>32</v>
@@ -1528,8 +1490,8 @@
       <c r="B4" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>175</v>
+      <c r="C4" s="3">
+        <v>1598</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>46</v>
@@ -1677,8 +1639,8 @@
       <c r="B5" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>176</v>
+      <c r="C5" s="4">
+        <v>1598</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>56</v>
@@ -1826,8 +1788,8 @@
       <c r="B6" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>177</v>
+      <c r="C6" s="3">
+        <v>1598</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>46</v>
@@ -1975,8 +1937,8 @@
       <c r="B7" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>178</v>
+      <c r="C7" s="4">
+        <v>1598</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>56</v>
@@ -2124,8 +2086,8 @@
       <c r="B8" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>179</v>
+      <c r="C8" s="3">
+        <v>1598</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>86</v>
@@ -2273,8 +2235,8 @@
       <c r="B9" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>180</v>
+      <c r="C9" s="4">
+        <v>1598</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>92</v>
@@ -2422,8 +2384,8 @@
       <c r="B10" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>181</v>
+      <c r="C10" s="3">
+        <v>1598</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>46</v>
@@ -2571,8 +2533,8 @@
       <c r="B11" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>182</v>
+      <c r="C11" s="4">
+        <v>1598</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>105</v>
@@ -2720,8 +2682,8 @@
       <c r="B12" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>183</v>
+      <c r="C12" s="3">
+        <v>1598</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>56</v>
@@ -2869,8 +2831,8 @@
       <c r="B13" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>184</v>
+      <c r="C13" s="2">
+        <v>1598</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>46</v>

</xml_diff>

<commit_message>
Aggiornate colonne al foglio superdettagli
</commit_message>
<xml_diff>
--- a/AAA Files for demo/Input files/Superdettagli_Light.xlsx
+++ b/AAA Files for demo/Input files/Superdettagli_Light.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\Lefo\Dev\3 GDPptGenerator\Solution\FilesEditor.Tests\TestFiles\SourceFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15C103FD-D92B-4CA3-8764-AC6847A80D37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4930B738-6B18-4893-8A2D-9939A45E4E7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="174">
   <si>
     <t>E005RD002</t>
   </si>
@@ -404,90 +404,24 @@
     <t>BBBB.0001</t>
   </si>
   <si>
-    <t>Sender Cost Center2</t>
-  </si>
-  <si>
-    <t>Personnel Number3</t>
-  </si>
-  <si>
-    <t>Last name First name4</t>
-  </si>
-  <si>
-    <t>Project Description5</t>
-  </si>
-  <si>
-    <t>WBS Element6</t>
-  </si>
-  <si>
-    <t>Network7</t>
-  </si>
-  <si>
-    <t>Operation/Activity8</t>
-  </si>
-  <si>
-    <t>Acct assgnt text9</t>
-  </si>
-  <si>
     <t>WBS Element - Project Definition (Text)</t>
   </si>
   <si>
     <t>Network descr</t>
   </si>
   <si>
-    <t>PROJ CODE10</t>
-  </si>
-  <si>
     <t>INT/EST</t>
   </si>
   <si>
-    <t>RAGGR X STRUTTURA 11</t>
-  </si>
-  <si>
     <t>MESE</t>
   </si>
   <si>
-    <t>Resp 2°liv12</t>
-  </si>
-  <si>
-    <t>CDC bdg13</t>
-  </si>
-  <si>
-    <t>Resp 1°liv14</t>
-  </si>
-  <si>
-    <t>Resp DT15</t>
-  </si>
-  <si>
-    <t>TIPO REP16</t>
-  </si>
-  <si>
     <t>Bus Area GDLT</t>
   </si>
   <si>
-    <t>Bus Area_217</t>
-  </si>
-  <si>
-    <t>tipo progetto18</t>
-  </si>
-  <si>
-    <t>Proj name19</t>
-  </si>
-  <si>
-    <t>machine code20</t>
-  </si>
-  <si>
-    <t>product area21</t>
-  </si>
-  <si>
-    <t>Resp del Prodotto22</t>
-  </si>
-  <si>
     <t>Area di bdg</t>
   </si>
   <si>
-    <t>Macchina23</t>
-  </si>
-  <si>
     <t>Sottotipo</t>
   </si>
   <si>
@@ -497,42 +431,6 @@
     <t>Quadrante</t>
   </si>
   <si>
-    <t>01.AAAA</t>
-  </si>
-  <si>
-    <t>02.AAAA</t>
-  </si>
-  <si>
-    <t>03.AAAA</t>
-  </si>
-  <si>
-    <t>04.AAAA</t>
-  </si>
-  <si>
-    <t>05.AAAA</t>
-  </si>
-  <si>
-    <t>06.AAAA</t>
-  </si>
-  <si>
-    <t>07.AAAA</t>
-  </si>
-  <si>
-    <t>08.AAAA</t>
-  </si>
-  <si>
-    <t>09.AAAA</t>
-  </si>
-  <si>
-    <t>10.AAAA</t>
-  </si>
-  <si>
-    <t>11.AAAA</t>
-  </si>
-  <si>
-    <t>12.AAAA</t>
-  </si>
-  <si>
     <t>Total</t>
   </si>
   <si>
@@ -555,6 +453,111 @@
   </si>
   <si>
     <t>Data Uscita GD</t>
+  </si>
+  <si>
+    <t>Sender Cost Center</t>
+  </si>
+  <si>
+    <t>Personnel Number</t>
+  </si>
+  <si>
+    <t>Last name First name</t>
+  </si>
+  <si>
+    <t>Project Description</t>
+  </si>
+  <si>
+    <t>WBS Element</t>
+  </si>
+  <si>
+    <t>Network</t>
+  </si>
+  <si>
+    <t>Operation/Activity</t>
+  </si>
+  <si>
+    <t>Acct assgnt text</t>
+  </si>
+  <si>
+    <t>PROJ CODE</t>
+  </si>
+  <si>
+    <t>Raggr. X Struttura</t>
+  </si>
+  <si>
+    <t>Resp 2°liv</t>
+  </si>
+  <si>
+    <t>CDC bdg</t>
+  </si>
+  <si>
+    <t>Resp 1°liv</t>
+  </si>
+  <si>
+    <t>Resp DT</t>
+  </si>
+  <si>
+    <t>TIPO REP</t>
+  </si>
+  <si>
+    <t>Bus Area_2</t>
+  </si>
+  <si>
+    <t>tipo progetto</t>
+  </si>
+  <si>
+    <t>Proj name</t>
+  </si>
+  <si>
+    <t>machine code</t>
+  </si>
+  <si>
+    <t>product area</t>
+  </si>
+  <si>
+    <t>Resp del Prodotto</t>
+  </si>
+  <si>
+    <t>Macchina</t>
+  </si>
+  <si>
+    <t>01.2025</t>
+  </si>
+  <si>
+    <t>02.2025</t>
+  </si>
+  <si>
+    <t>03.2025</t>
+  </si>
+  <si>
+    <t>04.2025</t>
+  </si>
+  <si>
+    <t>05.2025</t>
+  </si>
+  <si>
+    <t>06.2025</t>
+  </si>
+  <si>
+    <t>07.2025</t>
+  </si>
+  <si>
+    <t>08.2025</t>
+  </si>
+  <si>
+    <t>09.2025</t>
+  </si>
+  <si>
+    <t>10.2025</t>
+  </si>
+  <si>
+    <t>11.2025</t>
+  </si>
+  <si>
+    <t>12.2025</t>
+  </si>
+  <si>
+    <t>REP UT</t>
   </si>
 </sst>
 </file>
@@ -694,9 +697,9 @@
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -985,9 +988,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AY13"/>
+  <dimension ref="A1:AZ13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="AD1" workbookViewId="0">
+      <selection sqref="A1:AZ1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1028,164 +1033,168 @@
     <col min="49" max="49" width="27.140625" customWidth="1"/>
     <col min="50" max="50" width="17" customWidth="1"/>
     <col min="51" max="51" width="19.140625" customWidth="1"/>
+    <col min="52" max="52" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:51" ht="48" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:52" ht="48" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="I1" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="K1" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="M1" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="O1" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="U1" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="V1" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="AA1" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="AB1" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="AC1" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="AE1" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="AF1" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="AG1" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="AH1" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="AI1" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="AJ1" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="AK1" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="AL1" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="AM1" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="AR1" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="AS1" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="AT1" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="AU1" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="AV1" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="AW1" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="AX1" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="AY1" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="R1" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="V1" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="AB1" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="AF1" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="AG1" s="7" t="s">
-        <v>154</v>
-      </c>
-      <c r="AH1" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="AI1" s="7" t="s">
-        <v>156</v>
-      </c>
-      <c r="AJ1" s="7" t="s">
-        <v>157</v>
-      </c>
-      <c r="AK1" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="AL1" s="7" t="s">
-        <v>159</v>
-      </c>
-      <c r="AM1" s="7" t="s">
-        <v>160</v>
-      </c>
-      <c r="AN1" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="AO1" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="AP1" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="AQ1" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="AR1" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="AS1" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="AT1" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="AU1" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="AV1" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="AW1" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="AX1" s="8" t="s">
-        <v>171</v>
-      </c>
-      <c r="AY1" s="9" t="s">
-        <v>172</v>
+      <c r="AZ1" s="9" t="s">
+        <v>173</v>
       </c>
     </row>
-    <row r="2" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -1333,8 +1342,9 @@
         <v>29</v>
       </c>
       <c r="AY2" s="3"/>
+      <c r="AZ2" s="3"/>
     </row>
-    <row r="3" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>30</v>
       </c>
@@ -1482,8 +1492,9 @@
         <v>29</v>
       </c>
       <c r="AY3" s="4"/>
+      <c r="AZ3" s="4"/>
     </row>
-    <row r="4" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>44</v>
       </c>
@@ -1631,8 +1642,9 @@
         <v>29</v>
       </c>
       <c r="AY4" s="3"/>
+      <c r="AZ4" s="3"/>
     </row>
-    <row r="5" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>0</v>
       </c>
@@ -1780,8 +1792,9 @@
         <v>29</v>
       </c>
       <c r="AY5" s="4"/>
+      <c r="AZ5" s="4"/>
     </row>
-    <row r="6" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>69</v>
       </c>
@@ -1929,8 +1942,9 @@
         <v>29</v>
       </c>
       <c r="AY6" s="3"/>
+      <c r="AZ6" s="3"/>
     </row>
-    <row r="7" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>0</v>
       </c>
@@ -2078,8 +2092,9 @@
         <v>29</v>
       </c>
       <c r="AY7" s="4"/>
+      <c r="AZ7" s="4"/>
     </row>
-    <row r="8" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>85</v>
       </c>
@@ -2227,8 +2242,9 @@
         <v>29</v>
       </c>
       <c r="AY8" s="3"/>
+      <c r="AZ8" s="3"/>
     </row>
-    <row r="9" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>30</v>
       </c>
@@ -2376,8 +2392,9 @@
         <v>29</v>
       </c>
       <c r="AY9" s="4"/>
+      <c r="AZ9" s="4"/>
     </row>
-    <row r="10" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>44</v>
       </c>
@@ -2525,8 +2542,9 @@
         <v>29</v>
       </c>
       <c r="AY10" s="3"/>
+      <c r="AZ10" s="3"/>
     </row>
-    <row r="11" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>30</v>
       </c>
@@ -2674,8 +2692,9 @@
         <v>29</v>
       </c>
       <c r="AY11" s="4"/>
+      <c r="AZ11" s="4"/>
     </row>
-    <row r="12" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>110</v>
       </c>
@@ -2823,8 +2842,9 @@
         <v>29</v>
       </c>
       <c r="AY12" s="3"/>
+      <c r="AZ12" s="3"/>
     </row>
-    <row r="13" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:52" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>117</v>
       </c>
@@ -2972,6 +2992,7 @@
         <v>29</v>
       </c>
       <c r="AY13" s="2"/>
+      <c r="AZ13" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>